<commit_message>
First functional version of d13C processor...
</commit_message>
<xml_diff>
--- a/GCIRMS_d13C_Processor/GCIRMS C Template.xlsx
+++ b/GCIRMS_d13C_Processor/GCIRMS C Template.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9379E74E-A5D8-4B5E-8F4E-209163038A5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFBD39B5-F805-41EF-8212-50F86381C016}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="5" r:id="rId1"/>
@@ -681,18 +681,6 @@
     <t>initial_value</t>
   </si>
   <si>
-    <t>size_toosmall_peak_action</t>
-  </si>
-  <si>
-    <t>size_small_peak_action</t>
-  </si>
-  <si>
-    <t>size_normal_peak_action</t>
-  </si>
-  <si>
-    <t>size_large_peak_action</t>
-  </si>
-  <si>
     <t>acceptable_peak_units</t>
   </si>
   <si>
@@ -1266,6 +1254,18 @@
   </si>
   <si>
     <t>rArea.All</t>
+  </si>
+  <si>
+    <t>size_toosmall_peak_option</t>
+  </si>
+  <si>
+    <t>size_small_peak_option</t>
+  </si>
+  <si>
+    <t>size_normal_peak_option</t>
+  </si>
+  <si>
+    <t>size_large_peak_option</t>
   </si>
 </sst>
 </file>
@@ -2140,7 +2140,7 @@
         <v>138</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2178,35 +2178,35 @@
     </row>
     <row r="6" spans="1:3" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="33" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B6" s="34" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C6" s="35" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>145</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -2343,10 +2343,10 @@
         <v>19</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="L2" s="5" t="s">
         <v>48</v>
@@ -2367,7 +2367,7 @@
         <v>51</v>
       </c>
       <c r="T2" s="6" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="U2" s="6" t="str">
         <f>INDEX(U7:U8,MATCH(T10,T7:T8,0))</f>
@@ -2407,10 +2407,10 @@
         <v>19</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="L3" s="5" t="s">
         <v>48</v>
@@ -2431,10 +2431,10 @@
         <v>49</v>
       </c>
       <c r="T3" s="6" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="U3" s="6" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="V3" s="6">
         <v>46.7</v>
@@ -2470,10 +2470,10 @@
         <v>19</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="L4" s="5" t="s">
         <v>50</v>
@@ -2491,13 +2491,13 @@
         <v>46.7</v>
       </c>
       <c r="S4" s="7" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="T4" s="6" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="U4" s="6" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="V4" s="6">
         <f>V2-43.93</f>
@@ -2534,10 +2534,10 @@
         <v>19</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="L5" s="5" t="s">
         <v>50</v>
@@ -2585,7 +2585,7 @@
         <v>21</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="K6" s="5" t="s">
         <v>46</v>
@@ -2609,10 +2609,10 @@
         <v>99</v>
       </c>
       <c r="T6" s="7" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="U6" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.3">
@@ -2645,7 +2645,7 @@
         <v>21</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="K7" s="5" t="s">
         <v>46</v>
@@ -2670,10 +2670,10 @@
         <v>43.881666666666675</v>
       </c>
       <c r="T7" s="7" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="U7" s="6" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -2706,7 +2706,7 @@
         <v>1</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="K8" s="5" t="str">
         <f>Samples!$A$2</f>
@@ -2729,10 +2729,10 @@
       </c>
       <c r="S8" s="7"/>
       <c r="T8" s="37" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="U8" s="6" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.3">
@@ -2765,7 +2765,7 @@
         <v>1</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="K9" s="5" t="str">
         <f>Samples!$A$2</f>
@@ -2788,7 +2788,7 @@
       </c>
       <c r="S9" s="9"/>
       <c r="T9" s="39" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="U9" s="11"/>
     </row>
@@ -2822,7 +2822,7 @@
         <v>2</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="K10" s="5" t="str">
         <f>Samples!$A$3</f>
@@ -2845,7 +2845,7 @@
       </c>
       <c r="S10" s="9"/>
       <c r="T10" s="38" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="U10" s="11"/>
     </row>
@@ -2879,7 +2879,7 @@
         <v>2</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="K11" s="5" t="str">
         <f>Samples!$A$3</f>
@@ -2932,7 +2932,7 @@
         <v>3</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="K12" s="5" t="str">
         <f>Samples!$A$4</f>
@@ -2989,7 +2989,7 @@
         <v>3</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="K13" s="5" t="str">
         <f>Samples!$A$4</f>
@@ -3055,10 +3055,10 @@
         <v>19</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="K14" s="5" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="L14" s="5" t="s">
         <v>50</v>
@@ -3114,10 +3114,10 @@
         <v>19</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="L15" s="5" t="s">
         <v>50</v>
@@ -3173,7 +3173,7 @@
         <v>4</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="K16" s="5" t="str">
         <f>Samples!$A$5</f>
@@ -3239,7 +3239,7 @@
         <v>4</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="K17" s="5" t="str">
         <f>Samples!$A$5</f>
@@ -3299,10 +3299,10 @@
         <v>37</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="K18" s="5" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="L18" s="5" t="s">
         <v>39</v>
@@ -3358,10 +3358,10 @@
         <v>38</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="L19" s="5" t="s">
         <v>39</v>
@@ -3423,10 +3423,10 @@
         <v>39</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="L20" s="5" t="s">
         <v>39</v>
@@ -3482,10 +3482,10 @@
         <v>40</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="K21" s="5" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="L21" s="5" t="s">
         <v>39</v>
@@ -3541,10 +3541,10 @@
         <v>41</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="K22" s="5" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="L22" s="5" t="s">
         <v>39</v>
@@ -3605,10 +3605,10 @@
         <v>42</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="K23" s="5" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="L23" s="5" t="s">
         <v>39</v>
@@ -3663,10 +3663,10 @@
         <v>19</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="K24" s="5" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="L24" s="5" t="s">
         <v>50</v>
@@ -3721,10 +3721,10 @@
         <v>19</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="K25" s="5" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="L25" s="5" t="s">
         <v>50</v>
@@ -3785,7 +3785,7 @@
         <v>5</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="K26" s="5" t="str">
         <f>Samples!$A$6</f>
@@ -3844,7 +3844,7 @@
         <v>5</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="K27" s="5" t="str">
         <f>Samples!$A$6</f>
@@ -3903,7 +3903,7 @@
         <v>6</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="K28" s="5" t="str">
         <f>Samples!$A$7</f>
@@ -3966,7 +3966,7 @@
         <v>6</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="K29" s="5" t="str">
         <f>Samples!$A$7</f>
@@ -4025,7 +4025,7 @@
         <v>7</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="K30" s="5" t="str">
         <f>Samples!$A$8</f>
@@ -4084,7 +4084,7 @@
         <v>7</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="K31" s="5" t="str">
         <f>Samples!$A$8</f>
@@ -4106,11 +4106,11 @@
         <v>61.75</v>
       </c>
       <c r="V31" s="55" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="W31" s="56"/>
       <c r="X31" s="49" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="Y31" s="50"/>
     </row>
@@ -4144,10 +4144,10 @@
         <v>19</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="K32" s="5" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="L32" s="5" t="s">
         <v>50</v>
@@ -4199,10 +4199,10 @@
         <v>19</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="K33" s="5" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="L33" s="5" t="s">
         <v>50</v>
@@ -4254,7 +4254,7 @@
         <v>8</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="K34" s="5" t="str">
         <f>Samples!$A$9</f>
@@ -4314,7 +4314,7 @@
         <v>8</v>
       </c>
       <c r="J35" s="5" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="K35" s="5" t="str">
         <f>Samples!$A$9</f>
@@ -4370,7 +4370,7 @@
         <v>20</v>
       </c>
       <c r="J36" s="5" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="K36" s="5" t="s">
         <v>8</v>
@@ -4425,7 +4425,7 @@
         <v>20</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="K37" s="5" t="s">
         <v>8</v>
@@ -4476,7 +4476,7 @@
         <v>9</v>
       </c>
       <c r="J38" s="5" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="K38" s="5" t="str">
         <f>Samples!$A$10</f>
@@ -4528,7 +4528,7 @@
         <v>9</v>
       </c>
       <c r="J39" s="5" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="K39" s="5" t="str">
         <f>Samples!$A$10</f>
@@ -4580,10 +4580,10 @@
         <v>19</v>
       </c>
       <c r="J40" s="5" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="K40" s="5" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="L40" s="5" t="s">
         <v>50</v>
@@ -4631,10 +4631,10 @@
         <v>19</v>
       </c>
       <c r="J41" s="5" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="K41" s="5" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="L41" s="5" t="s">
         <v>50</v>
@@ -4682,7 +4682,7 @@
         <v>10</v>
       </c>
       <c r="J42" s="5" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="K42" s="5" t="str">
         <f>Samples!$A$11</f>
@@ -4734,7 +4734,7 @@
         <v>10</v>
       </c>
       <c r="J43" s="5" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="K43" s="5" t="str">
         <f>Samples!$A$11</f>
@@ -4786,7 +4786,7 @@
         <v>11</v>
       </c>
       <c r="J44" s="5" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="K44" s="5" t="str">
         <f>Samples!$A$12</f>
@@ -4838,7 +4838,7 @@
         <v>11</v>
       </c>
       <c r="J45" s="5" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="K45" s="5" t="str">
         <f>Samples!$A$12</f>
@@ -4890,7 +4890,7 @@
         <v>12</v>
       </c>
       <c r="J46" s="5" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="K46" s="5" t="str">
         <f>Samples!$A$13</f>
@@ -4942,7 +4942,7 @@
         <v>12</v>
       </c>
       <c r="J47" s="5" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="K47" s="5" t="str">
         <f>Samples!$A$13</f>
@@ -4994,10 +4994,10 @@
         <v>19</v>
       </c>
       <c r="J48" s="5" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="K48" s="5" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="L48" s="5" t="s">
         <v>50</v>
@@ -5045,10 +5045,10 @@
         <v>19</v>
       </c>
       <c r="J49" s="5" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="K49" s="5" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="L49" s="5" t="s">
         <v>50</v>
@@ -5089,20 +5089,20 @@
         <v>23</v>
       </c>
       <c r="H50" s="5" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="I50" s="5">
         <v>54</v>
       </c>
       <c r="J50" s="5" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="K50" s="5"/>
       <c r="L50" s="5"/>
       <c r="M50" s="5"/>
       <c r="N50" s="5"/>
       <c r="O50" s="5" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.3">
@@ -5582,7 +5582,7 @@
         <v>54</v>
       </c>
       <c r="H1" s="61" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="I1" s="17" t="s">
         <v>117</v>
@@ -5593,10 +5593,10 @@
     </row>
     <row r="2" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>45</v>
@@ -5613,15 +5613,15 @@
         <v>34</v>
       </c>
       <c r="J2" s="16" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>45</v>
@@ -5638,15 +5638,15 @@
         <v>21</v>
       </c>
       <c r="J3" s="16" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>45</v>
@@ -5668,10 +5668,10 @@
     </row>
     <row r="5" spans="1:10" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>45</v>
@@ -5693,10 +5693,10 @@
     </row>
     <row r="6" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>45</v>
@@ -5713,15 +5713,15 @@
         <v>3</v>
       </c>
       <c r="J6" s="16" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>45</v>
@@ -5743,10 +5743,10 @@
     </row>
     <row r="8" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>45</v>
@@ -5768,10 +5768,10 @@
     </row>
     <row r="9" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>45</v>
@@ -5787,10 +5787,10 @@
     </row>
     <row r="10" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>45</v>
@@ -5806,10 +5806,10 @@
     </row>
     <row r="11" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>45</v>
@@ -5825,10 +5825,10 @@
     </row>
     <row r="12" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A12" s="14" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>45</v>
@@ -5843,10 +5843,10 @@
     </row>
     <row r="13" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A13" s="14" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>45</v>
@@ -5983,13 +5983,13 @@
         <v>102</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="H1" s="79" t="s">
         <v>115</v>
@@ -6120,7 +6120,7 @@
         <v>102</v>
       </c>
       <c r="J5" s="16" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -6147,10 +6147,10 @@
       </c>
       <c r="H6" s="79"/>
       <c r="I6" s="16" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="J6" s="16" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -6176,7 +6176,7 @@
         <v>6</v>
       </c>
       <c r="I7" s="16" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="J7" s="16" t="s">
         <v>120</v>
@@ -6205,7 +6205,7 @@
         <v>5</v>
       </c>
       <c r="I8" s="16" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="J8" s="16" t="s">
         <v>121</v>
@@ -6329,13 +6329,13 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="D16" s="14">
         <v>1</v>
@@ -6352,7 +6352,7 @@
     </row>
     <row r="17" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="B17" s="15" t="s">
         <v>16</v>
@@ -6375,7 +6375,7 @@
     </row>
     <row r="18" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A18" s="15" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="B18" s="15" t="s">
         <v>17</v>
@@ -6398,7 +6398,7 @@
     </row>
     <row r="19" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A19" s="15" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="B19" s="15" t="s">
         <v>44</v>
@@ -6421,7 +6421,7 @@
     </row>
     <row r="20" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A20" s="15" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="B20" s="15" t="s">
         <v>45</v>
@@ -6444,7 +6444,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="B21" s="15" t="s">
         <v>47</v>
@@ -6467,7 +6467,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B22" s="15" t="s">
         <v>15</v>
@@ -6481,7 +6481,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B23" s="15" t="s">
         <v>16</v>
@@ -6495,7 +6495,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="15" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B24" s="15" t="s">
         <v>17</v>
@@ -6509,7 +6509,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="15" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B25" s="15" t="s">
         <v>44</v>
@@ -6523,7 +6523,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B26" s="15" t="s">
         <v>45</v>
@@ -6537,7 +6537,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="15" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B27" s="15" t="s">
         <v>47</v>
@@ -6551,10 +6551,10 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="C28" s="15" t="s">
         <v>11</v>
@@ -6565,10 +6565,10 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="C29" s="15" t="s">
         <v>11</v>
@@ -6675,10 +6675,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="C5" s="15" t="s">
         <v>75</v>
@@ -6694,7 +6694,7 @@
         <v>70</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="D6" s="22"/>
       <c r="E6" s="23"/>
@@ -6704,7 +6704,7 @@
         <v>63</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C7" s="15" t="s">
         <v>76</v>
@@ -6717,7 +6717,7 @@
         <v>64</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C8" s="15" t="s">
         <v>128</v>
@@ -6730,10 +6730,10 @@
         <v>65</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="D9" s="22"/>
       <c r="E9" s="22"/>
@@ -6746,7 +6746,7 @@
         <v>71</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="D10" s="22"/>
       <c r="E10" s="22"/>
@@ -6772,7 +6772,7 @@
         <v>72</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="D12" s="19"/>
       <c r="E12" s="19"/>
@@ -6802,13 +6802,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="B1" s="15" t="s">
         <v>66</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="D1" s="18" t="s">
         <v>117</v>
@@ -6819,7 +6819,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="B2" s="15">
         <v>768.2</v>
@@ -6828,15 +6828,15 @@
         <v>10</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E2" s="21" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="B3" s="15">
         <v>895.7</v>
@@ -6848,12 +6848,12 @@
         <v>66</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B4" s="15">
         <v>1217.5</v>
@@ -6862,15 +6862,15 @@
         <v>10</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B5" s="15">
         <v>1042.8</v>
@@ -6881,7 +6881,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="B6" s="15">
         <v>1357.2</v>
@@ -6892,7 +6892,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B7" s="15">
         <v>1373.3</v>
@@ -6903,7 +6903,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="B8" s="15">
         <v>1196.8</v>
@@ -6914,7 +6914,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B9" s="15">
         <v>1522.3</v>
@@ -6925,7 +6925,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="B10" s="15">
         <v>1350.6</v>
@@ -6936,7 +6936,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="B11" s="15">
         <v>1665.6</v>
@@ -6947,7 +6947,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="B12" s="15">
         <v>1816.6</v>
@@ -6958,7 +6958,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="B13" s="15">
         <v>2000.3</v>
@@ -6969,7 +6969,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B14" s="15">
         <v>1786.4</v>
@@ -6980,7 +6980,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="B15" s="15">
         <v>2243.6</v>
@@ -6991,7 +6991,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="B16" s="15">
         <v>2575.6</v>
@@ -7002,7 +7002,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="B17" s="15">
         <v>3034.2</v>
@@ -7013,7 +7013,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="B18" s="15">
         <v>40.1</v>
@@ -7024,7 +7024,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="B19" s="15">
         <v>89.9</v>
@@ -7035,7 +7035,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="B20" s="15">
         <v>139.6</v>
@@ -7053,7 +7053,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
@@ -7078,16 +7078,16 @@
         <v>10</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="G1" s="17" t="s">
         <v>117</v>
@@ -7156,10 +7156,10 @@
         <v>1</v>
       </c>
       <c r="G4" s="16" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="H4" s="16" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -7176,10 +7176,10 @@
         <v>1</v>
       </c>
       <c r="G5" s="16" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="H5" s="16" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -7196,7 +7196,7 @@
         <v>1</v>
       </c>
       <c r="G6" s="16" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="H6" s="16" t="s">
         <v>130</v>
@@ -7216,10 +7216,10 @@
         <v>1</v>
       </c>
       <c r="G7" s="16" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="H7" s="16" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -7316,8 +7316,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -7349,19 +7349,19 @@
     </row>
     <row r="2" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="29" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="D2" s="21" t="s">
         <v>78</v>
       </c>
       <c r="E2" s="21" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -7372,13 +7372,13 @@
         <v>79</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="D3" s="21" t="s">
         <v>146</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -7389,13 +7389,13 @@
         <v>80</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D4" s="21" t="s">
         <v>57</v>
       </c>
       <c r="E4" s="21" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -7406,18 +7406,18 @@
         <v>81</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="29" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B6" s="29" t="s">
         <v>93</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -7428,7 +7428,7 @@
         <v>82</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -7439,18 +7439,18 @@
         <v>83</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="29" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B9" s="29" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="C9" s="28" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -7458,78 +7458,78 @@
         <v>90</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="29" t="s">
-        <v>147</v>
+        <v>281</v>
       </c>
       <c r="B11" s="29" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="29" t="s">
-        <v>148</v>
+        <v>282</v>
       </c>
       <c r="B12" s="29" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="29" t="s">
-        <v>149</v>
+        <v>283</v>
       </c>
       <c r="B13" s="29" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="29" t="s">
-        <v>150</v>
+        <v>284</v>
       </c>
       <c r="B14" s="29" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="29" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B15" s="29" t="s">
         <v>83</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="29" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C16" s="28" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="29" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C17" s="28" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -7540,18 +7540,18 @@
         <v>84</v>
       </c>
       <c r="C18" s="28" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="29" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="B19" s="29" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="C19" s="28" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -7559,10 +7559,10 @@
         <v>92</v>
       </c>
       <c r="B20" s="29" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C20" s="28" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -7570,21 +7570,21 @@
         <v>92</v>
       </c>
       <c r="B21" s="29" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C21" s="28" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="29" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B22" s="29" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="C22" s="28" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Applied the last few commits for the d2H processor to d13C. Including: proper ref gas drift calculation, updated x-axis labels for size correction plots, and fixed step-wise scale normalization.
</commit_message>
<xml_diff>
--- a/GCIRMS_d13C_Processor/GCIRMS C Template.xlsx
+++ b/GCIRMS_d13C_Processor/GCIRMS C Template.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19982B0B-9DA4-4ABF-8DC4-7CA310F1F756}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{710B7CAE-0FFC-419F-98F5-B19FBF347DE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="5" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="921" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="926" uniqueCount="303">
   <si>
     <t>id1</t>
   </si>
@@ -1309,6 +1309,18 @@
   </si>
   <si>
     <t>Do not correct for derivative carbon.</t>
+  </si>
+  <si>
+    <t>Decide to indclude (or exclude) size standards when calculating control performance.</t>
+  </si>
+  <si>
+    <t>Include</t>
+  </si>
+  <si>
+    <t>size_for_control</t>
+  </si>
+  <si>
+    <t>Exclude</t>
   </si>
 </sst>
 </file>
@@ -1765,23 +1777,14 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1800,6 +1803,24 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1857,15 +1878,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3050,18 +3062,18 @@
         <v>61.75</v>
       </c>
       <c r="S13" s="8"/>
-      <c r="T13" s="55" t="s">
+      <c r="T13" s="58" t="s">
         <v>105</v>
       </c>
       <c r="U13" s="9"/>
-      <c r="V13" s="61" t="s">
+      <c r="V13" s="64" t="s">
         <v>103</v>
       </c>
-      <c r="W13" s="62"/>
-      <c r="X13" s="67" t="s">
+      <c r="W13" s="65"/>
+      <c r="X13" s="70" t="s">
         <v>104</v>
       </c>
-      <c r="Y13" s="68"/>
+      <c r="Y13" s="71"/>
       <c r="Z13" s="10"/>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.3">
@@ -3115,12 +3127,12 @@
         <v>46.7</v>
       </c>
       <c r="S14" s="8"/>
-      <c r="T14" s="56"/>
+      <c r="T14" s="59"/>
       <c r="U14" s="9"/>
-      <c r="V14" s="63"/>
-      <c r="W14" s="64"/>
-      <c r="X14" s="69"/>
-      <c r="Y14" s="70"/>
+      <c r="V14" s="66"/>
+      <c r="W14" s="67"/>
+      <c r="X14" s="72"/>
+      <c r="Y14" s="73"/>
       <c r="Z14" s="10"/>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.3">
@@ -3174,12 +3186,12 @@
         <v>46.7</v>
       </c>
       <c r="S15" s="8"/>
-      <c r="T15" s="57"/>
+      <c r="T15" s="60"/>
       <c r="U15" s="9"/>
-      <c r="V15" s="65"/>
-      <c r="W15" s="66"/>
-      <c r="X15" s="71"/>
-      <c r="Y15" s="72"/>
+      <c r="V15" s="68"/>
+      <c r="W15" s="69"/>
+      <c r="X15" s="74"/>
+      <c r="Y15" s="75"/>
       <c r="Z15" s="10"/>
     </row>
     <row r="16" spans="1:26" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -3234,18 +3246,18 @@
         <v>61.75</v>
       </c>
       <c r="S16" s="8"/>
-      <c r="T16" s="55" t="s">
+      <c r="T16" s="58" t="s">
         <v>99</v>
       </c>
       <c r="U16" s="9"/>
-      <c r="V16" s="43" t="s">
+      <c r="V16" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="W16" s="44"/>
-      <c r="X16" s="49" t="s">
+      <c r="W16" s="53"/>
+      <c r="X16" s="46" t="s">
         <v>106</v>
       </c>
-      <c r="Y16" s="50"/>
+      <c r="Y16" s="47"/>
       <c r="Z16" s="10"/>
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.3">
@@ -3300,12 +3312,12 @@
         <v>61.75</v>
       </c>
       <c r="S17" s="8"/>
-      <c r="T17" s="56"/>
+      <c r="T17" s="59"/>
       <c r="U17" s="9"/>
-      <c r="V17" s="45"/>
-      <c r="W17" s="46"/>
-      <c r="X17" s="51"/>
-      <c r="Y17" s="52"/>
+      <c r="V17" s="54"/>
+      <c r="W17" s="55"/>
+      <c r="X17" s="48"/>
+      <c r="Y17" s="49"/>
       <c r="Z17" s="10"/>
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.3">
@@ -3359,12 +3371,12 @@
         <v>46.7</v>
       </c>
       <c r="S18" s="8"/>
-      <c r="T18" s="57"/>
+      <c r="T18" s="60"/>
       <c r="U18" s="9"/>
-      <c r="V18" s="47"/>
-      <c r="W18" s="48"/>
-      <c r="X18" s="53"/>
-      <c r="Y18" s="54"/>
+      <c r="V18" s="56"/>
+      <c r="W18" s="57"/>
+      <c r="X18" s="50"/>
+      <c r="Y18" s="51"/>
       <c r="Z18" s="10"/>
     </row>
     <row r="19" spans="1:26" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -3418,18 +3430,18 @@
         <v>46.7</v>
       </c>
       <c r="S19" s="8"/>
-      <c r="T19" s="55" t="s">
+      <c r="T19" s="58" t="s">
         <v>100</v>
       </c>
       <c r="U19" s="9"/>
-      <c r="V19" s="43" t="s">
+      <c r="V19" s="52" t="s">
         <v>49</v>
       </c>
-      <c r="W19" s="44"/>
-      <c r="X19" s="49" t="s">
+      <c r="W19" s="53"/>
+      <c r="X19" s="46" t="s">
         <v>107</v>
       </c>
-      <c r="Y19" s="50"/>
+      <c r="Y19" s="47"/>
       <c r="Z19" s="10"/>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.3">
@@ -3483,12 +3495,12 @@
         <v>46.7</v>
       </c>
       <c r="S20" s="8"/>
-      <c r="T20" s="56"/>
+      <c r="T20" s="59"/>
       <c r="U20" s="9"/>
-      <c r="V20" s="45"/>
-      <c r="W20" s="46"/>
-      <c r="X20" s="51"/>
-      <c r="Y20" s="52"/>
+      <c r="V20" s="54"/>
+      <c r="W20" s="55"/>
+      <c r="X20" s="48"/>
+      <c r="Y20" s="49"/>
       <c r="Z20" s="10"/>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.3">
@@ -3542,12 +3554,12 @@
         <v>46.7</v>
       </c>
       <c r="S21" s="8"/>
-      <c r="T21" s="57"/>
+      <c r="T21" s="60"/>
       <c r="U21" s="9"/>
-      <c r="V21" s="47"/>
-      <c r="W21" s="48"/>
-      <c r="X21" s="53"/>
-      <c r="Y21" s="54"/>
+      <c r="V21" s="56"/>
+      <c r="W21" s="57"/>
+      <c r="X21" s="50"/>
+      <c r="Y21" s="51"/>
       <c r="Z21" s="10"/>
     </row>
     <row r="22" spans="1:26" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -3600,18 +3612,18 @@
         <f t="shared" si="2"/>
         <v>46.7</v>
       </c>
-      <c r="T22" s="55" t="s">
+      <c r="T22" s="58" t="s">
         <v>108</v>
       </c>
       <c r="U22" s="8"/>
-      <c r="V22" s="43" t="s">
+      <c r="V22" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="W22" s="44"/>
-      <c r="X22" s="49" t="s">
+      <c r="W22" s="53"/>
+      <c r="X22" s="46" t="s">
         <v>113</v>
       </c>
-      <c r="Y22" s="50"/>
+      <c r="Y22" s="47"/>
       <c r="Z22" s="10"/>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.3">
@@ -3664,12 +3676,12 @@
         <f t="shared" si="2"/>
         <v>46.7</v>
       </c>
-      <c r="T23" s="56"/>
+      <c r="T23" s="59"/>
       <c r="U23" s="8"/>
-      <c r="V23" s="45"/>
-      <c r="W23" s="46"/>
-      <c r="X23" s="51"/>
-      <c r="Y23" s="52"/>
+      <c r="V23" s="54"/>
+      <c r="W23" s="55"/>
+      <c r="X23" s="48"/>
+      <c r="Y23" s="49"/>
       <c r="Z23" s="10"/>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.3">
@@ -3722,12 +3734,12 @@
         <f t="shared" si="2"/>
         <v>46.7</v>
       </c>
-      <c r="T24" s="57"/>
+      <c r="T24" s="60"/>
       <c r="U24" s="8"/>
-      <c r="V24" s="47"/>
-      <c r="W24" s="48"/>
-      <c r="X24" s="53"/>
-      <c r="Y24" s="54"/>
+      <c r="V24" s="56"/>
+      <c r="W24" s="57"/>
+      <c r="X24" s="50"/>
+      <c r="Y24" s="51"/>
       <c r="Z24" s="10"/>
     </row>
     <row r="25" spans="1:26" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -3780,18 +3792,18 @@
         <f t="shared" si="2"/>
         <v>46.7</v>
       </c>
-      <c r="T25" s="58" t="s">
+      <c r="T25" s="61" t="s">
         <v>102</v>
       </c>
       <c r="U25" s="8"/>
-      <c r="V25" s="43" t="s">
+      <c r="V25" s="52" t="s">
         <v>109</v>
       </c>
-      <c r="W25" s="44"/>
-      <c r="X25" s="49" t="s">
+      <c r="W25" s="53"/>
+      <c r="X25" s="46" t="s">
         <v>110</v>
       </c>
-      <c r="Y25" s="50"/>
+      <c r="Y25" s="47"/>
       <c r="Z25" s="10"/>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.3">
@@ -3845,12 +3857,12 @@
         <f t="shared" si="2"/>
         <v>61.75</v>
       </c>
-      <c r="T26" s="59"/>
+      <c r="T26" s="62"/>
       <c r="U26" s="8"/>
-      <c r="V26" s="45"/>
-      <c r="W26" s="46"/>
-      <c r="X26" s="51"/>
-      <c r="Y26" s="52"/>
+      <c r="V26" s="54"/>
+      <c r="W26" s="55"/>
+      <c r="X26" s="48"/>
+      <c r="Y26" s="49"/>
       <c r="Z26" s="10"/>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.3">
@@ -3904,12 +3916,12 @@
         <f t="shared" si="2"/>
         <v>61.75</v>
       </c>
-      <c r="T27" s="59"/>
+      <c r="T27" s="62"/>
       <c r="U27" s="8"/>
-      <c r="V27" s="47"/>
-      <c r="W27" s="48"/>
-      <c r="X27" s="53"/>
-      <c r="Y27" s="54"/>
+      <c r="V27" s="56"/>
+      <c r="W27" s="57"/>
+      <c r="X27" s="50"/>
+      <c r="Y27" s="51"/>
       <c r="Z27" s="10"/>
     </row>
     <row r="28" spans="1:26" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -3963,16 +3975,16 @@
         <f t="shared" si="2"/>
         <v>61.75</v>
       </c>
-      <c r="T28" s="59"/>
+      <c r="T28" s="62"/>
       <c r="U28" s="8"/>
-      <c r="V28" s="43" t="s">
+      <c r="V28" s="52" t="s">
         <v>39</v>
       </c>
-      <c r="W28" s="44"/>
-      <c r="X28" s="49" t="s">
+      <c r="W28" s="53"/>
+      <c r="X28" s="46" t="s">
         <v>111</v>
       </c>
-      <c r="Y28" s="50"/>
+      <c r="Y28" s="47"/>
       <c r="Z28" s="10"/>
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.3">
@@ -4026,12 +4038,12 @@
         <f t="shared" si="2"/>
         <v>61.75</v>
       </c>
-      <c r="T29" s="59"/>
+      <c r="T29" s="62"/>
       <c r="U29" s="8"/>
-      <c r="V29" s="45"/>
-      <c r="W29" s="46"/>
-      <c r="X29" s="51"/>
-      <c r="Y29" s="52"/>
+      <c r="V29" s="54"/>
+      <c r="W29" s="55"/>
+      <c r="X29" s="48"/>
+      <c r="Y29" s="49"/>
       <c r="Z29" s="10"/>
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.3">
@@ -4085,12 +4097,12 @@
         <f t="shared" si="2"/>
         <v>61.75</v>
       </c>
-      <c r="T30" s="60"/>
+      <c r="T30" s="63"/>
       <c r="U30" s="8"/>
-      <c r="V30" s="47"/>
-      <c r="W30" s="48"/>
-      <c r="X30" s="53"/>
-      <c r="Y30" s="54"/>
+      <c r="V30" s="56"/>
+      <c r="W30" s="57"/>
+      <c r="X30" s="50"/>
+      <c r="Y30" s="51"/>
       <c r="Z30" s="10"/>
     </row>
     <row r="31" spans="1:26" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -4144,14 +4156,14 @@
         <f t="shared" si="2"/>
         <v>61.75</v>
       </c>
-      <c r="V31" s="43" t="s">
+      <c r="V31" s="52" t="s">
         <v>186</v>
       </c>
-      <c r="W31" s="44"/>
-      <c r="X31" s="49" t="s">
+      <c r="W31" s="53"/>
+      <c r="X31" s="46" t="s">
         <v>187</v>
       </c>
-      <c r="Y31" s="50"/>
+      <c r="Y31" s="47"/>
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
@@ -4203,10 +4215,10 @@
         <f t="shared" si="2"/>
         <v>46.7</v>
       </c>
-      <c r="V32" s="45"/>
-      <c r="W32" s="46"/>
-      <c r="X32" s="51"/>
-      <c r="Y32" s="52"/>
+      <c r="V32" s="54"/>
+      <c r="W32" s="55"/>
+      <c r="X32" s="48"/>
+      <c r="Y32" s="49"/>
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
@@ -4258,10 +4270,10 @@
         <f t="shared" si="2"/>
         <v>46.7</v>
       </c>
-      <c r="V33" s="47"/>
-      <c r="W33" s="48"/>
-      <c r="X33" s="53"/>
-      <c r="Y33" s="54"/>
+      <c r="V33" s="56"/>
+      <c r="W33" s="57"/>
+      <c r="X33" s="50"/>
+      <c r="Y33" s="51"/>
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
@@ -4314,14 +4326,14 @@
         <f t="shared" si="2"/>
         <v>61.75</v>
       </c>
-      <c r="V34" s="43" t="s">
+      <c r="V34" s="52" t="s">
         <v>51</v>
       </c>
-      <c r="W34" s="44"/>
-      <c r="X34" s="49" t="s">
+      <c r="W34" s="53"/>
+      <c r="X34" s="46" t="s">
         <v>112</v>
       </c>
-      <c r="Y34" s="50"/>
+      <c r="Y34" s="47"/>
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
@@ -4374,10 +4386,10 @@
         <f t="shared" si="2"/>
         <v>61.75</v>
       </c>
-      <c r="V35" s="45"/>
-      <c r="W35" s="46"/>
-      <c r="X35" s="51"/>
-      <c r="Y35" s="52"/>
+      <c r="V35" s="54"/>
+      <c r="W35" s="55"/>
+      <c r="X35" s="48"/>
+      <c r="Y35" s="49"/>
     </row>
     <row r="36" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
@@ -4429,10 +4441,10 @@
         <f t="shared" si="2"/>
         <v>46.7</v>
       </c>
-      <c r="V36" s="47"/>
-      <c r="W36" s="48"/>
-      <c r="X36" s="53"/>
-      <c r="Y36" s="54"/>
+      <c r="V36" s="56"/>
+      <c r="W36" s="57"/>
+      <c r="X36" s="50"/>
+      <c r="Y36" s="51"/>
     </row>
     <row r="37" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
@@ -5542,11 +5554,6 @@
     <sortCondition descending="1" ref="A41:A46"/>
   </sortState>
   <mergeCells count="21">
-    <mergeCell ref="X22:Y24"/>
-    <mergeCell ref="V25:W27"/>
-    <mergeCell ref="X25:Y27"/>
-    <mergeCell ref="V28:W30"/>
-    <mergeCell ref="X28:Y30"/>
     <mergeCell ref="V34:W36"/>
     <mergeCell ref="X34:Y36"/>
     <mergeCell ref="T13:T15"/>
@@ -5563,6 +5570,11 @@
     <mergeCell ref="V31:W33"/>
     <mergeCell ref="X31:Y33"/>
     <mergeCell ref="V22:W24"/>
+    <mergeCell ref="X22:Y24"/>
+    <mergeCell ref="V25:W27"/>
+    <mergeCell ref="X25:Y27"/>
+    <mergeCell ref="V28:W30"/>
+    <mergeCell ref="X28:Y30"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations disablePrompts="1" count="1">
@@ -5620,7 +5632,7 @@
       <c r="G1" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="H1" s="55" t="s">
+      <c r="H1" s="58" t="s">
         <v>192</v>
       </c>
       <c r="I1" s="16" t="s">
@@ -5645,7 +5657,7 @@
       </c>
       <c r="F2" s="41"/>
       <c r="G2" s="42"/>
-      <c r="H2" s="56"/>
+      <c r="H2" s="59"/>
       <c r="I2" s="15" t="s">
         <v>34</v>
       </c>
@@ -5668,7 +5680,7 @@
       </c>
       <c r="F3" s="41"/>
       <c r="G3" s="42"/>
-      <c r="H3" s="56"/>
+      <c r="H3" s="59"/>
       <c r="I3" s="15" t="s">
         <v>21</v>
       </c>
@@ -5691,7 +5703,7 @@
       </c>
       <c r="F4" s="41"/>
       <c r="G4" s="42"/>
-      <c r="H4" s="56"/>
+      <c r="H4" s="59"/>
       <c r="I4" s="15" t="s">
         <v>1</v>
       </c>
@@ -5714,7 +5726,7 @@
       </c>
       <c r="F5" s="41"/>
       <c r="G5" s="42"/>
-      <c r="H5" s="56"/>
+      <c r="H5" s="59"/>
       <c r="I5" s="15" t="s">
         <v>2</v>
       </c>
@@ -5737,7 +5749,7 @@
       </c>
       <c r="F6" s="41"/>
       <c r="G6" s="42"/>
-      <c r="H6" s="56"/>
+      <c r="H6" s="59"/>
       <c r="I6" s="15" t="s">
         <v>3</v>
       </c>
@@ -5760,7 +5772,7 @@
       </c>
       <c r="F7" s="41"/>
       <c r="G7" s="42"/>
-      <c r="H7" s="56"/>
+      <c r="H7" s="59"/>
       <c r="I7" s="15" t="s">
         <v>53</v>
       </c>
@@ -5783,7 +5795,7 @@
       </c>
       <c r="F8" s="41"/>
       <c r="G8" s="42"/>
-      <c r="H8" s="57"/>
+      <c r="H8" s="60"/>
       <c r="I8" s="15" t="s">
         <v>54</v>
       </c>
@@ -6006,7 +6018,7 @@
       <c r="G1" s="14" t="s">
         <v>251</v>
       </c>
-      <c r="H1" s="73" t="s">
+      <c r="H1" s="76" t="s">
         <v>114</v>
       </c>
       <c r="I1" s="16" t="s">
@@ -6038,7 +6050,7 @@
       <c r="G2" s="14">
         <v>65</v>
       </c>
-      <c r="H2" s="73"/>
+      <c r="H2" s="76"/>
       <c r="I2" s="15" t="s">
         <v>34</v>
       </c>
@@ -6068,7 +6080,7 @@
       <c r="G3" s="14">
         <v>5</v>
       </c>
-      <c r="H3" s="73"/>
+      <c r="H3" s="76"/>
       <c r="I3" s="15" t="s">
         <v>10</v>
       </c>
@@ -6098,7 +6110,7 @@
       <c r="G4" s="14">
         <v>3</v>
       </c>
-      <c r="H4" s="73" t="s">
+      <c r="H4" s="76" t="s">
         <v>115</v>
       </c>
       <c r="I4" s="15" t="s">
@@ -6130,7 +6142,7 @@
       <c r="G5" s="14">
         <v>5</v>
       </c>
-      <c r="H5" s="73"/>
+      <c r="H5" s="76"/>
       <c r="I5" s="15" t="s">
         <v>101</v>
       </c>
@@ -6160,7 +6172,7 @@
       <c r="G6" s="14">
         <v>5</v>
       </c>
-      <c r="H6" s="73"/>
+      <c r="H6" s="76"/>
       <c r="I6" s="15" t="s">
         <v>249</v>
       </c>
@@ -7504,10 +7516,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:K22"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -7518,10 +7530,10 @@
     <col min="4" max="4" width="24.6640625" style="25" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="97.77734375" style="25" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="8.88671875" style="25"/>
-    <col min="8" max="8" width="52.88671875" style="76" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="62.33203125" style="76" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="70.77734375" style="76" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.6640625" style="76" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="52.88671875" style="45" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="62.33203125" style="45" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="70.77734375" style="45" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" style="45" bestFit="1" customWidth="1"/>
     <col min="12" max="16384" width="8.88671875" style="25"/>
   </cols>
   <sheetData>
@@ -7541,16 +7553,16 @@
       <c r="E1" s="30" t="s">
         <v>104</v>
       </c>
-      <c r="H1" s="74" t="s">
+      <c r="H1" s="43" t="s">
         <v>286</v>
       </c>
-      <c r="I1" s="74" t="s">
+      <c r="I1" s="43" t="s">
         <v>287</v>
       </c>
-      <c r="J1" s="74" t="s">
+      <c r="J1" s="43" t="s">
         <v>288</v>
       </c>
-      <c r="K1" s="74"/>
+      <c r="K1" s="43"/>
     </row>
     <row r="2" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="27" t="s">
@@ -7568,10 +7580,10 @@
       <c r="E2" s="19" t="s">
         <v>170</v>
       </c>
-      <c r="H2" s="75" t="s">
+      <c r="H2" s="44" t="s">
         <v>222</v>
       </c>
-      <c r="I2" s="76" t="s">
+      <c r="I2" s="45" t="s">
         <v>289</v>
       </c>
     </row>
@@ -7591,13 +7603,13 @@
       <c r="E3" s="19" t="s">
         <v>171</v>
       </c>
-      <c r="H3" s="76" t="s">
+      <c r="H3" s="45" t="s">
         <v>79</v>
       </c>
-      <c r="I3" s="76" t="s">
+      <c r="I3" s="45" t="s">
         <v>80</v>
       </c>
-      <c r="J3" s="76" t="s">
+      <c r="J3" s="45" t="s">
         <v>81</v>
       </c>
     </row>
@@ -7617,13 +7629,13 @@
       <c r="E4" s="19" t="s">
         <v>172</v>
       </c>
-      <c r="H4" s="76" t="s">
+      <c r="H4" s="45" t="s">
         <v>80</v>
       </c>
-      <c r="I4" s="76" t="s">
+      <c r="I4" s="45" t="s">
         <v>79</v>
       </c>
-      <c r="J4" s="76" t="s">
+      <c r="J4" s="45" t="s">
         <v>81</v>
       </c>
     </row>
@@ -7637,13 +7649,13 @@
       <c r="C5" s="26" t="s">
         <v>156</v>
       </c>
-      <c r="H5" s="76" t="s">
+      <c r="H5" s="45" t="s">
         <v>81</v>
       </c>
-      <c r="I5" s="76" t="s">
+      <c r="I5" s="45" t="s">
         <v>79</v>
       </c>
-      <c r="J5" s="76" t="s">
+      <c r="J5" s="45" t="s">
         <v>80</v>
       </c>
     </row>
@@ -7657,13 +7669,13 @@
       <c r="C6" s="26" t="s">
         <v>157</v>
       </c>
-      <c r="H6" s="76" t="s">
+      <c r="H6" s="45" t="s">
         <v>92</v>
       </c>
-      <c r="I6" s="76" t="s">
+      <c r="I6" s="45" t="s">
         <v>290</v>
       </c>
-      <c r="J6" s="76" t="s">
+      <c r="J6" s="45" t="s">
         <v>291</v>
       </c>
     </row>
@@ -7694,10 +7706,10 @@
       <c r="H8" s="27" t="s">
         <v>284</v>
       </c>
-      <c r="I8" s="76" t="s">
+      <c r="I8" s="45" t="s">
         <v>83</v>
       </c>
-      <c r="J8" s="76" t="s">
+      <c r="J8" s="45" t="s">
         <v>292</v>
       </c>
     </row>
@@ -7714,10 +7726,10 @@
       <c r="H9" s="27" t="s">
         <v>285</v>
       </c>
-      <c r="I9" s="76" t="s">
+      <c r="I9" s="45" t="s">
         <v>293</v>
       </c>
-      <c r="J9" s="76" t="s">
+      <c r="J9" s="45" t="s">
         <v>294</v>
       </c>
     </row>
@@ -7743,10 +7755,10 @@
       <c r="H11" s="27" t="s">
         <v>149</v>
       </c>
-      <c r="I11" s="76" t="s">
+      <c r="I11" s="45" t="s">
         <v>284</v>
       </c>
-      <c r="J11" s="76" t="s">
+      <c r="J11" s="45" t="s">
         <v>295</v>
       </c>
     </row>
@@ -7763,7 +7775,7 @@
       <c r="H12" s="27" t="s">
         <v>150</v>
       </c>
-      <c r="I12" s="76" t="s">
+      <c r="I12" s="45" t="s">
         <v>284</v>
       </c>
     </row>
@@ -7780,7 +7792,7 @@
       <c r="H13" s="27" t="s">
         <v>150</v>
       </c>
-      <c r="I13" s="76" t="s">
+      <c r="I13" s="45" t="s">
         <v>284</v>
       </c>
     </row>
@@ -7797,7 +7809,7 @@
       <c r="H14" s="27" t="s">
         <v>151</v>
       </c>
-      <c r="I14" s="76" t="s">
+      <c r="I14" s="45" t="s">
         <v>284</v>
       </c>
       <c r="J14" s="27" t="s">
@@ -7817,7 +7829,7 @@
       <c r="H15" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="I15" s="76" t="s">
+      <c r="I15" s="45" t="s">
         <v>292</v>
       </c>
     </row>
@@ -7830,7 +7842,7 @@
       </c>
       <c r="H16" s="27"/>
     </row>
-    <row r="17" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="27" t="s">
         <v>148</v>
       </c>
@@ -7839,87 +7851,103 @@
       </c>
       <c r="H17" s="27"/>
     </row>
-    <row r="18" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="27" t="s">
+        <v>301</v>
+      </c>
+      <c r="B18" s="27" t="s">
+        <v>300</v>
+      </c>
+      <c r="C18" s="26" t="s">
+        <v>299</v>
+      </c>
+      <c r="H18" s="25" t="s">
+        <v>300</v>
+      </c>
+      <c r="I18" s="25" t="s">
+        <v>302</v>
+      </c>
+      <c r="J18" s="25"/>
+      <c r="K18" s="25"/>
+    </row>
+    <row r="19" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="B18" s="27" t="s">
+      <c r="B19" s="27" t="s">
         <v>268</v>
       </c>
-      <c r="C18" s="26" t="s">
+      <c r="C19" s="26" t="s">
         <v>168</v>
       </c>
-      <c r="H18" s="27" t="s">
+      <c r="H19" s="27" t="s">
         <v>268</v>
       </c>
-      <c r="I18" s="76" t="s">
+      <c r="I19" s="45" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="27" t="s">
+    <row r="20" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="27" t="s">
         <v>236</v>
       </c>
-      <c r="B19" s="27" t="s">
+      <c r="B20" s="27" t="s">
         <v>269</v>
       </c>
-      <c r="C19" s="26" t="s">
+      <c r="C20" s="26" t="s">
         <v>237</v>
       </c>
-      <c r="H19" s="27"/>
-    </row>
-    <row r="20" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="27" t="s">
-        <v>91</v>
-      </c>
-      <c r="B20" s="27" t="s">
-        <v>152</v>
-      </c>
-      <c r="C20" s="26" t="s">
-        <v>169</v>
-      </c>
       <c r="H20" s="27"/>
     </row>
-    <row r="21" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="27" t="s">
         <v>91</v>
       </c>
       <c r="B21" s="27" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C21" s="26" t="s">
         <v>169</v>
       </c>
       <c r="H21" s="27"/>
     </row>
-    <row r="22" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="B22" s="27" t="s">
+        <v>153</v>
+      </c>
+      <c r="C22" s="26" t="s">
+        <v>169</v>
+      </c>
+      <c r="H22" s="27"/>
+    </row>
+    <row r="23" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="27" t="s">
         <v>225</v>
       </c>
-      <c r="B22" s="27" t="s">
+      <c r="B23" s="27" t="s">
         <v>263</v>
       </c>
-      <c r="C22" s="26" t="s">
+      <c r="C23" s="26" t="s">
         <v>261</v>
       </c>
-      <c r="H22" s="27" t="s">
+      <c r="H23" s="27" t="s">
         <v>263</v>
       </c>
-      <c r="I22" s="76" t="s">
+      <c r="I23" s="45" t="s">
         <v>297</v>
       </c>
-      <c r="J22" s="76" t="s">
+      <c r="J23" s="45" t="s">
         <v>298</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2 B4 B5 B6 B7 B8 B9 B11 B12 B13 B14 B15 B18 B22" xr:uid="{ABA6ABBA-A0A8-4936-BAC4-D2A59DFB82C2}">
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11:B15 B18:B19 B23 B2:B9" xr:uid="{ABA6ABBA-A0A8-4936-BAC4-D2A59DFB82C2}">
       <formula1>H2:J2</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{BA0EDCDF-F767-450B-B886-C45536472629}">
-      <formula1>H3:J3</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>